<commit_message>
Ready To Run n2
</commit_message>
<xml_diff>
--- a/ipa_2/myUtils/games.xlsx
+++ b/ipa_2/myUtils/games.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A07083A-EFFA-4D59-93A8-1CC639737B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C345C863-1F67-45DF-98A9-F61D1D050C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +582,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -597,19 +597,19 @@
         <v>19</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K4">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -670,7 +670,7 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -685,10 +685,10 @@
         <v>19</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I6">
         <v>10</v>

</xml_diff>